<commit_message>
update test excel files
</commit_message>
<xml_diff>
--- a/xls/GlobalSetting.xlsx
+++ b/xls/GlobalSetting.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,28 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projs\avatar-ava-xls2lua\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9854BBA1-F028-4F02-9A71-2B04E3AE036A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250B9C13-4400-4B96-853F-61AC78E057ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24075" yWindow="2445" windowWidth="21600" windowHeight="13095"/>
+    <workbookView xWindow="5295" yWindow="2310" windowWidth="21600" windowHeight="13095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="output_GlobalSetting" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="70">
   <si>
     <t>Type</t>
   </si>
@@ -224,17 +215,37 @@
   </si>
   <si>
     <t>描述</t>
+  </si>
+  <si>
+    <t>Test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Function</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lua</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>function() print(12) end</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -242,6 +253,14 @@
       <sz val="9"/>
       <name val="等线"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -264,13 +283,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -546,26 +568,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="24.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="42.42578125" style="1" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="17.28515625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.125" style="1"/>
+    <col min="2" max="2" width="24.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.25" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="42.375" style="1" customWidth="1"/>
+    <col min="6" max="7" width="9.125" style="1"/>
+    <col min="8" max="8" width="17.25" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>60</v>
       </c>
@@ -581,8 +603,11 @@
       <c r="E1" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>60</v>
       </c>
@@ -598,8 +623,11 @@
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -612,11 +640,14 @@
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="E3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -632,8 +663,11 @@
       <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -650,7 +684,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -667,7 +701,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -684,7 +718,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -701,7 +735,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -718,7 +752,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -735,7 +769,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>8</v>
       </c>
@@ -752,7 +786,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>9</v>
       </c>
@@ -769,7 +803,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -786,7 +820,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>11</v>
       </c>
@@ -803,7 +837,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>12</v>
       </c>
@@ -820,7 +854,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>13</v>
       </c>
@@ -837,7 +871,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>14</v>
       </c>
@@ -854,7 +888,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>15</v>
       </c>
@@ -871,7 +905,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>16</v>
       </c>
@@ -888,7 +922,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>17</v>
       </c>
@@ -905,7 +939,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>18</v>
       </c>
@@ -922,7 +956,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>19</v>
       </c>
@@ -939,7 +973,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>20</v>
       </c>
@@ -956,7 +990,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>21</v>
       </c>
@@ -973,7 +1007,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>22</v>
       </c>
@@ -990,7 +1024,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>23</v>
       </c>

</xml_diff>